<commit_message>
major changes to support multiple chats
</commit_message>
<xml_diff>
--- a/data/popular_accounts_manually_validated_with_sv.xlsx
+++ b/data/popular_accounts_manually_validated_with_sv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlotan/code/university/personal_llm/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C3F5D3-C13D-BA45-AD74-75AAC4334F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BDF121-D0DA-084D-B2F0-2172335837DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20000" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="🎤Singers" sheetId="2" r:id="rId1"/>
@@ -14015,9 +14015,6 @@
     <t>12044602</t>
   </si>
   <si>
-    <t>Arnold</t>
-  </si>
-  <si>
     <t>Former Mr. Olympia, Conan, Terminator, and Governor of California. I killed the Predator. I told you I'd be back. Sign up for my newsletter:</t>
   </si>
   <si>
@@ -14275,6 +14272,9 @@
   </si>
   <si>
     <t>Ice T</t>
+  </si>
+  <si>
+    <t>Arnold Schwarzenegger</t>
   </si>
 </sst>
 </file>
@@ -14364,7 +14364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -15348,7 +15348,7 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>2274</v>
+        <v>2273</v>
       </c>
       <c r="E22" t="s">
         <v>1261</v>
@@ -15569,7 +15569,7 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>2271</v>
+        <v>2270</v>
       </c>
       <c r="E29" t="s">
         <v>1297</v>
@@ -15761,7 +15761,7 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>2272</v>
+        <v>2271</v>
       </c>
       <c r="E35" t="s">
         <v>1333</v>
@@ -15825,7 +15825,7 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>2273</v>
+        <v>2272</v>
       </c>
       <c r="E37" t="s">
         <v>1344</v>
@@ -18721,7 +18721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:AF92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="186" zoomScaleNormal="186" workbookViewId="0">
+    <sheetView zoomScale="186" zoomScaleNormal="186" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -21767,11 +21767,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21839,22 +21839,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>2235</v>
+      </c>
+      <c r="B4" t="s">
         <v>2236</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>2237</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>2238</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>2239</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2240</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -21939,22 +21939,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>2250</v>
+      </c>
+      <c r="B9" t="s">
         <v>2251</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>2252</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>2253</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>2254</v>
-      </c>
-      <c r="F9" t="s">
-        <v>2255</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -21979,22 +21979,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>2265</v>
+      </c>
+      <c r="B11" t="s">
         <v>2266</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>2267</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>2268</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>2269</v>
-      </c>
-      <c r="F11" t="s">
-        <v>2270</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -22039,22 +22039,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B14" t="s">
         <v>2261</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
         <v>2262</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>2263</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>2264</v>
-      </c>
-      <c r="F14" t="s">
-        <v>2265</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -22136,22 +22136,22 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>2255</v>
+      </c>
+      <c r="B19" t="s">
         <v>2256</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
         <v>2257</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>2258</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>2259</v>
-      </c>
-      <c r="F19" t="s">
-        <v>2260</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -22205,33 +22205,33 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
+        <v>2274</v>
+      </c>
+      <c r="E22" t="s">
         <v>2233</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>2234</v>
-      </c>
-      <c r="F22" t="s">
-        <v>2235</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>2240</v>
+      </c>
+      <c r="B23" t="s">
         <v>2241</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
         <v>2242</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>2243</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>2244</v>
-      </c>
-      <c r="F23" t="s">
-        <v>2245</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -22296,22 +22296,22 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>2245</v>
+      </c>
+      <c r="B27" t="s">
         <v>2246</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
         <v>2247</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>2248</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>2249</v>
-      </c>
-      <c r="F27" t="s">
-        <v>2250</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>